<commit_message>
Final Pushes Before Publication
</commit_message>
<xml_diff>
--- a/Data Analysis/Boost and Etho/All Clusters In Dataset/A2.xlsx
+++ b/Data Analysis/Boost and Etho/All Clusters In Dataset/A2.xlsx
@@ -238,9 +238,9 @@
   <dimension ref="A1:C57"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="true"/>
-    <col min="2" max="2" width="13.42578125" customWidth="true"/>
-    <col min="3" max="3" width="14.42578125" customWidth="true"/>
+    <col min="1" max="1" width="20.6015625" customWidth="true"/>
+    <col min="2" max="2" width="13.37890625" customWidth="true"/>
+    <col min="3" max="3" width="14.37890625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>